<commit_message>
mas arreglos de casos de uso
</commit_message>
<xml_diff>
--- a/Medotologia.xlsx
+++ b/Medotologia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDa\Desktop\Projecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7D03A0-CB36-4DA7-B019-45DABC22B586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3F2F51-4FDC-4FC2-A268-AD74453133D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guía" sheetId="10" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="295">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1031,6 +1031,15 @@
   </si>
   <si>
     <t>P3</t>
+  </si>
+  <si>
+    <t>Añadir una direccion</t>
+  </si>
+  <si>
+    <t>Para que el repartidor sepa donde enviarlo</t>
+  </si>
+  <si>
+    <t>Para saber cuanto producto se descuenta del inventario</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2058,37 +2067,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2179,6 +2187,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2194,15 +2226,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2215,21 +2238,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2242,11 +2250,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7627,11 +7633,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:3" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="163" t="s">
+      <c r="A2" s="160" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="165"/>
+      <c r="B2" s="161"/>
+      <c r="C2" s="162"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="123" t="s">
@@ -8247,19 +8253,19 @@
       <c r="A73" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="B73" s="166" t="s">
+      <c r="B73" s="163" t="s">
         <v>121</v>
       </c>
-      <c r="C73" s="167"/>
+      <c r="C73" s="164"/>
     </row>
     <row r="74" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="B74" s="168" t="s">
+      <c r="B74" s="165" t="s">
         <v>187</v>
       </c>
-      <c r="C74" s="169"/>
+      <c r="C74" s="166"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="111" t="s">
@@ -8274,64 +8280,64 @@
       <c r="A76" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="B76" s="161" t="s">
+      <c r="B76" s="167" t="s">
         <v>140</v>
       </c>
-      <c r="C76" s="162"/>
+      <c r="C76" s="168"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="B77" s="161" t="s">
+      <c r="B77" s="167" t="s">
         <v>141</v>
       </c>
-      <c r="C77" s="162"/>
+      <c r="C77" s="168"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="112" t="s">
         <v>171</v>
       </c>
-      <c r="B78" s="161" t="s">
+      <c r="B78" s="167" t="s">
         <v>145</v>
       </c>
-      <c r="C78" s="162"/>
+      <c r="C78" s="168"/>
     </row>
     <row r="79" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="112" t="s">
         <v>172</v>
       </c>
-      <c r="B79" s="161" t="s">
+      <c r="B79" s="167" t="s">
         <v>142</v>
       </c>
-      <c r="C79" s="162"/>
+      <c r="C79" s="168"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="112" t="s">
         <v>173</v>
       </c>
-      <c r="B80" s="161" t="s">
+      <c r="B80" s="167" t="s">
         <v>143</v>
       </c>
-      <c r="C80" s="162"/>
+      <c r="C80" s="168"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="112" t="s">
         <v>174</v>
       </c>
-      <c r="B81" s="161" t="s">
+      <c r="B81" s="167" t="s">
         <v>144</v>
       </c>
-      <c r="C81" s="162"/>
+      <c r="C81" s="168"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="112" t="s">
         <v>175</v>
       </c>
-      <c r="B82" s="161" t="s">
+      <c r="B82" s="167" t="s">
         <v>176</v>
       </c>
-      <c r="C82" s="162"/>
+      <c r="C82" s="168"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="112"/>
@@ -8351,10 +8357,10 @@
       <c r="A85" s="112" t="s">
         <v>178</v>
       </c>
-      <c r="B85" s="161" t="s">
+      <c r="B85" s="167" t="s">
         <v>157</v>
       </c>
-      <c r="C85" s="162"/>
+      <c r="C85" s="168"/>
     </row>
     <row r="86" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="112" t="s">
@@ -8369,19 +8375,19 @@
       <c r="A87" s="112" t="s">
         <v>180</v>
       </c>
-      <c r="B87" s="161" t="s">
+      <c r="B87" s="167" t="s">
         <v>147</v>
       </c>
-      <c r="C87" s="162"/>
+      <c r="C87" s="168"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="112" t="s">
         <v>181</v>
       </c>
-      <c r="B88" s="161" t="s">
+      <c r="B88" s="167" t="s">
         <v>149</v>
       </c>
-      <c r="C88" s="162"/>
+      <c r="C88" s="168"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="112"/>
@@ -8401,28 +8407,28 @@
       <c r="A91" s="112" t="s">
         <v>183</v>
       </c>
-      <c r="B91" s="161" t="s">
+      <c r="B91" s="167" t="s">
         <v>155</v>
       </c>
-      <c r="C91" s="162"/>
+      <c r="C91" s="168"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B92" s="161" t="s">
+      <c r="B92" s="167" t="s">
         <v>158</v>
       </c>
-      <c r="C92" s="162"/>
+      <c r="C92" s="168"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="B93" s="161" t="s">
+      <c r="B93" s="167" t="s">
         <v>156</v>
       </c>
-      <c r="C93" s="162"/>
+      <c r="C93" s="168"/>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="116"/>
@@ -8431,22 +8437,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
     <mergeCell ref="B88:C88"/>
     <mergeCell ref="B91:C91"/>
     <mergeCell ref="B92:C92"/>
     <mergeCell ref="B93:C93"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8458,8 +8464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8471,20 +8477,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="173" t="s">
+      <c r="A2" s="172" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
     </row>
     <row r="3" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="149" t="s">
@@ -8501,7 +8507,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="174" t="s">
+      <c r="B4" s="173" t="s">
         <v>264</v>
       </c>
       <c r="C4" s="152" t="s">
@@ -8512,7 +8518,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="175"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="153" t="s">
         <v>266</v>
       </c>
@@ -8521,7 +8527,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="175"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="152" t="s">
         <v>262</v>
       </c>
@@ -8530,7 +8536,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="175"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="153" t="s">
         <v>278</v>
       </c>
@@ -8539,7 +8545,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="175"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="153" t="s">
         <v>273</v>
       </c>
@@ -8548,17 +8554,17 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="175"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="153"/>
       <c r="D9" s="153"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="176"/>
+      <c r="B10" s="175"/>
       <c r="C10" s="153"/>
       <c r="D10" s="153"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="171" t="s">
+      <c r="B11" s="170" t="s">
         <v>269</v>
       </c>
       <c r="C11" s="154" t="s">
@@ -8569,7 +8575,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="172"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="154" t="s">
         <v>280</v>
       </c>
@@ -8578,7 +8584,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="172"/>
+      <c r="B13" s="171"/>
       <c r="C13" s="154" t="s">
         <v>279</v>
       </c>
@@ -8587,7 +8593,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="176" t="s">
         <v>282</v>
       </c>
       <c r="C14" s="155" t="s">
@@ -8598,7 +8604,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="178"/>
+      <c r="B15" s="177"/>
       <c r="C15" s="155" t="s">
         <v>249</v>
       </c>
@@ -8607,7 +8613,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="178"/>
+      <c r="B16" s="177"/>
       <c r="C16" s="155" t="s">
         <v>287</v>
       </c>
@@ -8616,7 +8622,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="178"/>
+      <c r="B17" s="177"/>
       <c r="C17" s="155" t="s">
         <v>289</v>
       </c>
@@ -8625,7 +8631,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="178"/>
+      <c r="B18" s="177"/>
       <c r="C18" s="155" t="s">
         <v>245</v>
       </c>
@@ -8634,12 +8640,12 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="179"/>
+      <c r="B19" s="178"/>
       <c r="C19" s="158"/>
       <c r="D19" s="158"/>
     </row>
     <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="180" t="s">
+      <c r="B20" s="179" t="s">
         <v>283</v>
       </c>
       <c r="C20" s="156" t="s">
@@ -8650,7 +8656,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="180"/>
+      <c r="B21" s="179"/>
       <c r="C21" s="156" t="s">
         <v>285</v>
       </c>
@@ -8659,26 +8665,34 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="180"/>
-      <c r="C22" s="160" t="s">
+      <c r="B22" s="179"/>
+      <c r="C22" s="159" t="s">
         <v>272</v>
       </c>
-      <c r="D22" s="160" t="s">
+      <c r="D22" s="159" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="180"/>
-      <c r="C23" s="159"/>
-      <c r="D23" s="159"/>
+      <c r="B23" s="179"/>
+      <c r="C23" s="220" t="s">
+        <v>245</v>
+      </c>
+      <c r="D23" s="220" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="180"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
+      <c r="B24" s="179"/>
+      <c r="C24" s="220" t="s">
+        <v>292</v>
+      </c>
+      <c r="D24" s="220" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="25" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="170" t="s">
+      <c r="B25" s="169" t="s">
         <v>270</v>
       </c>
       <c r="C25" s="157" t="s">
@@ -8689,7 +8703,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="170"/>
+      <c r="B26" s="169"/>
       <c r="C26" s="157" t="s">
         <v>254</v>
       </c>
@@ -8698,7 +8712,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="170"/>
+      <c r="B27" s="169"/>
       <c r="C27" s="157" t="s">
         <v>256</v>
       </c>
@@ -8707,7 +8721,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="170"/>
+      <c r="B28" s="169"/>
       <c r="C28" s="157" t="s">
         <v>258</v>
       </c>
@@ -8716,7 +8730,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="170"/>
+      <c r="B29" s="169"/>
       <c r="C29" s="157"/>
       <c r="D29" s="157"/>
     </row>
@@ -8793,13 +8807,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="181" t="s">
+      <c r="A1" s="180" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
@@ -8812,48 +8826,48 @@
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="17"/>
-      <c r="H2" s="193" t="s">
+      <c r="H2" s="192" t="s">
         <v>191</v>
       </c>
-      <c r="I2" s="194"/>
-      <c r="J2" s="195"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="194"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="181" t="s">
         <v>198</v>
       </c>
-      <c r="D3" s="185" t="s">
+      <c r="D3" s="184" t="s">
         <v>196</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="7"/>
-      <c r="H3" s="191" t="s">
+      <c r="H3" s="190" t="s">
         <v>192</v>
       </c>
-      <c r="I3" s="191" t="s">
+      <c r="I3" s="190" t="s">
         <v>193</v>
       </c>
-      <c r="J3" s="191" t="s">
+      <c r="J3" s="190" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="183"/>
+      <c r="B4" s="182"/>
       <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="186"/>
+      <c r="D4" s="185"/>
       <c r="F4" s="7"/>
-      <c r="H4" s="192"/>
-      <c r="I4" s="192"/>
-      <c r="J4" s="192"/>
+      <c r="H4" s="191"/>
+      <c r="I4" s="191"/>
+      <c r="J4" s="191"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="183"/>
-      <c r="D5" s="186"/>
+      <c r="B5" s="182"/>
+      <c r="D5" s="185"/>
       <c r="E5" s="22" t="s">
         <v>1</v>
       </c>
@@ -8866,8 +8880,8 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
-      <c r="B6" s="184"/>
-      <c r="D6" s="187"/>
+      <c r="B6" s="183"/>
+      <c r="D6" s="186"/>
       <c r="F6" s="7"/>
       <c r="H6" s="131"/>
       <c r="I6" s="131"/>
@@ -8885,7 +8899,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="D8" s="188" t="s">
+      <c r="D8" s="187" t="s">
         <v>197</v>
       </c>
       <c r="E8" s="22"/>
@@ -8896,7 +8910,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="D9" s="189"/>
+      <c r="D9" s="188"/>
       <c r="F9" s="7"/>
       <c r="H9" s="132"/>
       <c r="I9" s="132"/>
@@ -8904,7 +8918,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="D10" s="189"/>
+      <c r="D10" s="188"/>
       <c r="E10" s="22"/>
       <c r="F10" s="7"/>
       <c r="H10" s="132"/>
@@ -8913,7 +8927,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="D11" s="190"/>
+      <c r="D11" s="189"/>
       <c r="F11" s="7"/>
       <c r="H11" s="132"/>
       <c r="I11" s="132"/>
@@ -8947,7 +8961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="36" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="36" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AC52" sqref="AC52"/>
     </sheetView>
   </sheetViews>
@@ -9315,18 +9329,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="195" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9661,13 +9675,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="197" t="s">
+      <c r="A2" s="196" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
+      <c r="B2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
       <c r="F2" s="52"/>
       <c r="G2" t="s">
         <v>0</v>
@@ -9714,14 +9728,14 @@
       <c r="F4" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="198"/>
+      <c r="G4" s="197"/>
       <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="40"/>
       <c r="D5" s="34"/>
       <c r="F5" s="27"/>
-      <c r="G5" s="199"/>
+      <c r="G5" s="198"/>
       <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -10119,24 +10133,11 @@
       <c r="H47" s="27"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="221"/>
-      <c r="B48" s="222"/>
-      <c r="C48" s="223"/>
-      <c r="D48" s="223"/>
-      <c r="E48" s="223"/>
-      <c r="F48" s="224"/>
-      <c r="G48" s="223"/>
-      <c r="H48" s="223"/>
+      <c r="F48" s="104"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="221"/>
-      <c r="B49" s="222"/>
-      <c r="C49" s="223"/>
-      <c r="D49" s="223"/>
-      <c r="E49" s="223"/>
-      <c r="F49" s="224"/>
-      <c r="G49" s="225"/>
-      <c r="H49" s="223"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="57"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C50" s="33"/>
@@ -10242,114 +10243,95 @@
       <c r="F64" s="139"/>
       <c r="H64" s="27"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C65" s="33"/>
       <c r="D65" s="34"/>
       <c r="F65" s="139"/>
       <c r="H65" s="27"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C66" s="41"/>
       <c r="D66" s="42"/>
       <c r="F66" s="139"/>
       <c r="H66" s="27"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C67" s="33"/>
       <c r="D67" s="34"/>
       <c r="F67" s="139"/>
       <c r="H67" s="27"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C68" s="41"/>
       <c r="D68" s="42"/>
       <c r="F68" s="139"/>
       <c r="H68" s="27"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="221"/>
-      <c r="B69" s="222"/>
-      <c r="C69" s="223"/>
-      <c r="D69" s="223"/>
-      <c r="E69" s="223"/>
-      <c r="F69" s="224"/>
-      <c r="G69" s="223"/>
-      <c r="H69" s="223"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="221"/>
-      <c r="B70" s="222"/>
-      <c r="C70" s="223"/>
-      <c r="D70" s="223"/>
-      <c r="E70" s="223"/>
-      <c r="F70" s="224"/>
-      <c r="G70" s="225"/>
-      <c r="H70" s="223"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="221"/>
-      <c r="B71" s="222"/>
-      <c r="C71" s="223"/>
-      <c r="D71" s="223"/>
-      <c r="E71" s="223"/>
-      <c r="F71" s="224"/>
-      <c r="G71" s="225"/>
-      <c r="H71" s="223"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F69" s="104"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F70" s="104"/>
+      <c r="G70" s="57"/>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F71" s="104"/>
+      <c r="G71" s="57"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C72" s="33"/>
       <c r="D72" s="34"/>
       <c r="F72" s="139"/>
       <c r="G72" s="57"/>
       <c r="H72" s="27"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C73" s="33"/>
       <c r="D73" s="34"/>
       <c r="F73" s="139"/>
       <c r="G73" s="99"/>
       <c r="H73" s="27"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C74" s="33"/>
       <c r="D74" s="34"/>
       <c r="F74" s="139"/>
       <c r="H74" s="27"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C75" s="41"/>
       <c r="D75" s="42"/>
       <c r="F75" s="139"/>
       <c r="G75" s="24"/>
       <c r="H75" s="27"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C76" s="33"/>
       <c r="D76" s="34"/>
       <c r="F76" s="139"/>
       <c r="G76" s="100"/>
       <c r="H76" s="27"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C77" s="33"/>
       <c r="D77" s="34"/>
       <c r="F77" s="139"/>
       <c r="G77" s="100"/>
       <c r="H77" s="27"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="33"/>
       <c r="D78" s="34"/>
       <c r="F78" s="139"/>
       <c r="H78" s="27"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C79" s="41"/>
       <c r="D79" s="42"/>
       <c r="F79" s="139"/>
       <c r="H79" s="27"/>
     </row>
-    <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="33"/>
       <c r="D80" s="34"/>
       <c r="F80" s="139"/>
@@ -11114,48 +11096,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="215" t="s">
+      <c r="B1" s="199" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
-      <c r="G1" s="215"/>
-      <c r="H1" s="215"/>
-      <c r="I1" s="215"/>
-      <c r="J1" s="215"/>
-      <c r="K1" s="215"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="199"/>
+      <c r="I1" s="199"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="199"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="216"/>
-      <c r="J2" s="216"/>
-      <c r="K2" s="216"/>
-      <c r="L2" s="216"/>
-      <c r="M2" s="216"/>
-      <c r="N2" s="216"/>
-      <c r="O2" s="216"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="I2" s="200"/>
+      <c r="J2" s="200"/>
+      <c r="K2" s="200"/>
+      <c r="L2" s="200"/>
+      <c r="M2" s="200"/>
+      <c r="N2" s="200"/>
+      <c r="O2" s="200"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="53"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="209"/>
-      <c r="I4" s="205"/>
-      <c r="J4" s="206"/>
-      <c r="K4" s="207"/>
-      <c r="M4" s="205"/>
-      <c r="N4" s="206"/>
-      <c r="O4" s="207"/>
+      <c r="E4" s="212"/>
+      <c r="F4" s="213"/>
+      <c r="I4" s="201"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="203"/>
+      <c r="M4" s="201"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="203"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="53"/>
-      <c r="E5" s="203"/>
-      <c r="F5" s="204"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="211"/>
       <c r="I5" s="75"/>
       <c r="J5" s="76"/>
       <c r="K5" s="77"/>
@@ -11212,22 +11194,22 @@
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="53"/>
-      <c r="E11" s="208"/>
-      <c r="F11" s="209"/>
+      <c r="E11" s="212"/>
+      <c r="F11" s="213"/>
       <c r="I11" s="79"/>
       <c r="J11" s="73"/>
       <c r="K11" s="74"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="53"/>
-      <c r="E12" s="203"/>
-      <c r="F12" s="204"/>
+      <c r="E12" s="210"/>
+      <c r="F12" s="211"/>
       <c r="I12" s="80"/>
       <c r="J12" s="81"/>
       <c r="K12" s="82"/>
-      <c r="M12" s="205"/>
-      <c r="N12" s="206"/>
-      <c r="O12" s="207"/>
+      <c r="M12" s="201"/>
+      <c r="N12" s="202"/>
+      <c r="O12" s="203"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="53"/>
@@ -11262,9 +11244,9 @@
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" s="78"/>
       <c r="F16" s="71"/>
-      <c r="I16" s="205"/>
-      <c r="J16" s="206"/>
-      <c r="K16" s="207"/>
+      <c r="I16" s="201"/>
+      <c r="J16" s="202"/>
+      <c r="K16" s="203"/>
       <c r="M16" s="78"/>
       <c r="N16" s="70"/>
       <c r="O16" s="71"/>
@@ -11333,14 +11315,14 @@
       <c r="I23" s="80"/>
       <c r="J23" s="81"/>
       <c r="K23" s="82"/>
-      <c r="M23" s="205"/>
-      <c r="N23" s="206"/>
-      <c r="O23" s="207"/>
+      <c r="M23" s="201"/>
+      <c r="N23" s="202"/>
+      <c r="O23" s="203"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="50"/>
-      <c r="E24" s="208"/>
-      <c r="F24" s="209"/>
+      <c r="E24" s="212"/>
+      <c r="F24" s="213"/>
       <c r="I24" s="83"/>
       <c r="J24" s="84"/>
       <c r="K24" s="85"/>
@@ -11350,8 +11332,8 @@
     </row>
     <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="56"/>
-      <c r="E25" s="203"/>
-      <c r="F25" s="204"/>
+      <c r="E25" s="210"/>
+      <c r="F25" s="211"/>
       <c r="I25" s="86"/>
       <c r="J25" s="87"/>
       <c r="K25" s="88"/>
@@ -11371,9 +11353,9 @@
       <c r="B27" s="50"/>
       <c r="E27" s="78"/>
       <c r="F27" s="71"/>
-      <c r="I27" s="205"/>
-      <c r="J27" s="206"/>
-      <c r="K27" s="207"/>
+      <c r="I27" s="201"/>
+      <c r="J27" s="202"/>
+      <c r="K27" s="203"/>
       <c r="M27" s="78"/>
       <c r="N27" s="70"/>
       <c r="O27" s="71"/>
@@ -11420,8 +11402,8 @@
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="50"/>
-      <c r="E32" s="208"/>
-      <c r="F32" s="209"/>
+      <c r="E32" s="212"/>
+      <c r="F32" s="213"/>
       <c r="I32" s="2"/>
       <c r="M32" s="86"/>
       <c r="N32" s="87"/>
@@ -11429,17 +11411,17 @@
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="55"/>
-      <c r="E33" s="210"/>
-      <c r="F33" s="211"/>
+      <c r="E33" s="214"/>
+      <c r="F33" s="215"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="50"/>
       <c r="E34" s="75"/>
       <c r="F34" s="77"/>
-      <c r="I34" s="205"/>
-      <c r="J34" s="206"/>
-      <c r="K34" s="207"/>
+      <c r="I34" s="201"/>
+      <c r="J34" s="202"/>
+      <c r="K34" s="203"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="50"/>
@@ -11448,9 +11430,9 @@
       <c r="I35" s="97"/>
       <c r="J35" s="76"/>
       <c r="K35" s="77"/>
-      <c r="M35" s="205"/>
-      <c r="N35" s="206"/>
-      <c r="O35" s="207"/>
+      <c r="M35" s="201"/>
+      <c r="N35" s="202"/>
+      <c r="O35" s="203"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="50"/>
@@ -11515,9 +11497,9 @@
       <c r="I42" s="83"/>
       <c r="J42" s="84"/>
       <c r="K42" s="85"/>
-      <c r="M42" s="205"/>
-      <c r="N42" s="206"/>
-      <c r="O42" s="207"/>
+      <c r="M42" s="201"/>
+      <c r="N42" s="202"/>
+      <c r="O42" s="203"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" s="55"/>
@@ -11546,18 +11528,18 @@
     </row>
     <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="47"/>
-      <c r="I46" s="212"/>
-      <c r="J46" s="213"/>
-      <c r="K46" s="214"/>
+      <c r="I46" s="204"/>
+      <c r="J46" s="205"/>
+      <c r="K46" s="206"/>
       <c r="M46" s="89"/>
       <c r="N46" s="90"/>
       <c r="O46" s="91"/>
     </row>
     <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="47"/>
-      <c r="I47" s="200"/>
-      <c r="J47" s="201"/>
-      <c r="K47" s="202"/>
+      <c r="I47" s="207"/>
+      <c r="J47" s="208"/>
+      <c r="K47" s="209"/>
     </row>
     <row r="48" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="47"/>
@@ -11572,15 +11554,15 @@
       <c r="B50" s="47"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I51" s="212"/>
-      <c r="J51" s="213"/>
-      <c r="K51" s="214"/>
+      <c r="I51" s="204"/>
+      <c r="J51" s="205"/>
+      <c r="K51" s="206"/>
     </row>
     <row r="52" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="84"/>
-      <c r="I52" s="200"/>
-      <c r="J52" s="201"/>
-      <c r="K52" s="202"/>
+      <c r="I52" s="207"/>
+      <c r="J52" s="208"/>
+      <c r="K52" s="209"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="84"/>
@@ -11740,16 +11722,6 @@
     <sortCondition ref="B61:B98"/>
   </sortState>
   <mergeCells count="23">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="E2:O2"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="M12:O12"/>
     <mergeCell ref="I52:K52"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="M4:O4"/>
@@ -11763,6 +11735,16 @@
     <mergeCell ref="M42:O42"/>
     <mergeCell ref="I47:K47"/>
     <mergeCell ref="I51:K51"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="E2:O2"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="M12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11797,38 +11779,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="220" t="s">
+      <c r="B1" s="219" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="219"/>
+      <c r="H1" s="219"/>
+      <c r="I1" s="219"/>
+      <c r="J1" s="219"/>
+      <c r="K1" s="219"/>
+      <c r="L1" s="219"/>
+      <c r="M1" s="219"/>
+      <c r="N1" s="219"/>
+      <c r="O1" s="219"/>
+      <c r="P1" s="219"/>
     </row>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="217"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="219"/>
-      <c r="F3" s="217"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="219"/>
-      <c r="J3" s="217"/>
-      <c r="K3" s="218"/>
-      <c r="L3" s="219"/>
-      <c r="N3" s="217"/>
-      <c r="O3" s="218"/>
-      <c r="P3" s="219"/>
+      <c r="B3" s="216"/>
+      <c r="C3" s="217"/>
+      <c r="D3" s="218"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="217"/>
+      <c r="H3" s="218"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="217"/>
+      <c r="L3" s="218"/>
+      <c r="N3" s="216"/>
+      <c r="O3" s="217"/>
+      <c r="P3" s="218"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="80" t="s">
@@ -11882,9 +11864,9 @@
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="217"/>
-      <c r="C8" s="218"/>
-      <c r="D8" s="219"/>
+      <c r="B8" s="216"/>
+      <c r="C8" s="217"/>
+      <c r="D8" s="218"/>
       <c r="F8" s="67"/>
       <c r="G8" s="61"/>
       <c r="H8" s="62"/>
@@ -11911,17 +11893,17 @@
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="217"/>
-      <c r="K12" s="218"/>
-      <c r="L12" s="219"/>
-      <c r="N12" s="217"/>
-      <c r="O12" s="218"/>
-      <c r="P12" s="219"/>
+      <c r="J12" s="216"/>
+      <c r="K12" s="217"/>
+      <c r="L12" s="218"/>
+      <c r="N12" s="216"/>
+      <c r="O12" s="217"/>
+      <c r="P12" s="218"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="217"/>
-      <c r="C13" s="218"/>
-      <c r="D13" s="219"/>
+      <c r="B13" s="216"/>
+      <c r="C13" s="217"/>
+      <c r="D13" s="218"/>
       <c r="J13" s="80"/>
       <c r="K13" s="81"/>
       <c r="L13" s="82"/>
@@ -11942,9 +11924,9 @@
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="D15" s="7"/>
-      <c r="F15" s="217"/>
-      <c r="G15" s="218"/>
-      <c r="H15" s="219"/>
+      <c r="F15" s="216"/>
+      <c r="G15" s="217"/>
+      <c r="H15" s="218"/>
       <c r="J15" s="54"/>
       <c r="K15" s="13"/>
       <c r="L15" s="14"/>

</xml_diff>